<commit_message>
Ready to release commit
</commit_message>
<xml_diff>
--- a/Javista.AttributesFactory/Template/Attributes_Template.xlsx
+++ b/Javista.AttributesFactory/Template/Attributes_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttouzard\OneDrive - JAVISTA\PROJETS\Javista.AttributesFactory\Javista.AttributesFactory\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\T\Github\Javista.AttributesFactory\Javista.AttributesFactory\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_EE9268DBFADD019849EC07B0AE64FCABAA71FFF0" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{72B2C534-9C20-4702-85A0-84113EDADA02}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020AD067-1315-437B-9BC1-CCF6F4DA5C24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
   <si>
     <t>Description</t>
   </si>
@@ -1191,41 +1191,35 @@
     <t>Multiselect OptionSet</t>
   </si>
   <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Floating</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Phonetic guide</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
     <t>Only fill white background cells. Grey background cells become white depending on attribute type. 
-From default template, only rows 4 to 17 embed validation logic. Extend last row to add more attributes</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Ignore</t>
-  </si>
-  <si>
-    <t>Decimal</t>
-  </si>
-  <si>
-    <t>Floating</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Phonetic guide</t>
-  </si>
-  <si>
-    <t>Version number</t>
-  </si>
-  <si>
-    <t>Locale</t>
-  </si>
-  <si>
-    <t>redfgd</t>
-  </si>
-  <si>
-    <t>new_nreztertre</t>
+From default template, only three first rows embed validation logic. Insert new rows before last row to add more attributes</t>
   </si>
 </sst>
 </file>
@@ -1538,12 +1532,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1598,13 +1589,85 @@
       <alignment vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1628,16 +1691,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
@@ -1649,89 +1712,13 @@
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="78">
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -2836,7 +2823,7 @@
   <dimension ref="A1:BD5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
@@ -2853,300 +2840,296 @@
     <col min="10" max="10" width="10.1328125" customWidth="1"/>
     <col min="11" max="11" width="14.1328125" customWidth="1"/>
     <col min="12" max="12" width="20.3984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="12.53125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="4.1328125" style="9" customWidth="1" collapsed="1"/>
-    <col min="16" max="18" width="10.86328125" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="4.1328125" customWidth="1"/>
-    <col min="20" max="21" width="10.86328125" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="4.1328125" customWidth="1"/>
-    <col min="23" max="25" width="10.86328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="4.1328125" customWidth="1" collapsed="1"/>
-    <col min="27" max="29" width="10.86328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="4.1328125" customWidth="1" collapsed="1"/>
-    <col min="31" max="33" width="10.86328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="4.1328125" customWidth="1" collapsed="1"/>
-    <col min="35" max="37" width="10.86328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="4.1328125" customWidth="1" collapsed="1"/>
-    <col min="39" max="40" width="10.86328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="4.1328125" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="22.3984375" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="10.86328125" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="18.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="18" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="18.53125" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="19.3984375" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="55" width="10.86328125" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="4.1328125" customWidth="1"/>
+    <col min="13" max="13" width="11" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="12.53125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="16" max="18" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="23" max="25" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="27" max="29" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="31" max="33" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="35" max="37" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="39" max="40" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.33203125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="22.3984375" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="18.33203125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="18" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="18.53125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="19.3984375" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="55" width="10.86328125" style="21" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="4.1328125" style="21" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:56" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="51"/>
+      <c r="O1" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="58"/>
+      <c r="V1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA1" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE1" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI1" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM1" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="39"/>
+      <c r="AS1" s="39"/>
+      <c r="AT1" s="39"/>
+      <c r="AU1" s="39"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="39"/>
+      <c r="AX1" s="39"/>
+      <c r="AY1" s="39"/>
+      <c r="AZ1" s="39"/>
+      <c r="BA1" s="39"/>
+      <c r="BB1" s="39"/>
+      <c r="BC1" s="40"/>
+      <c r="BD1" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="W1" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA1" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE1" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI1" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM1" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP1" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
-      <c r="AW1" s="53"/>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
-      <c r="AZ1" s="53"/>
-      <c r="BA1" s="53"/>
-      <c r="BB1" s="53"/>
-      <c r="BC1" s="54"/>
-      <c r="BD1" s="40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:56" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="60"/>
+      <c r="P2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="11" t="s">
+      <c r="S2" s="62"/>
+      <c r="T2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="43"/>
-      <c r="W2" s="6" t="s">
+      <c r="V2" s="29"/>
+      <c r="W2" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="6" t="s">
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AB2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AC2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD2" s="47"/>
-      <c r="AE2" s="6" t="s">
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AF2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AG2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="6" t="s">
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AK2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="5" t="s">
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AN2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="5" t="s">
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AR2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AS2" s="5" t="s">
+      <c r="AS2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AT2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AU2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AV2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AW2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AX2" s="5" t="s">
+      <c r="AX2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AY2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AZ2" s="5" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BA2" s="5" t="s">
+      <c r="BA2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BB2" s="5" t="s">
+      <c r="BB2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BC2" s="5" t="s">
+      <c r="BC2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BD2" s="41"/>
+      <c r="BD2" s="27"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="A3" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="22" t="s">
@@ -3164,112 +3147,117 @@
       <c r="L3" s="1">
         <v>100</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="s">
+      <c r="N3" s="7"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="13"/>
-      <c r="U3" t="s">
+      <c r="R3" s="6"/>
+      <c r="S3" s="12"/>
+      <c r="U3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="14"/>
-      <c r="W3" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="X3">
-        <v>-2147483647</v>
-      </c>
-      <c r="Y3">
+      <c r="X3" s="21">
+        <v>-2147483648</v>
+      </c>
+      <c r="Y3" s="21">
         <v>2147483647</v>
       </c>
-      <c r="Z3" s="15"/>
-      <c r="AA3">
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="21">
         <v>2</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="21">
         <v>0</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="21">
         <v>1000000000</v>
       </c>
-      <c r="AD3" s="16"/>
-      <c r="AE3">
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="21">
         <v>2</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="21">
         <v>-100000000000</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="21">
         <v>100000000000</v>
       </c>
-      <c r="AH3" s="17"/>
-      <c r="AI3">
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="21">
         <v>2</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="21">
         <v>-922337203685477</v>
       </c>
-      <c r="AK3">
+      <c r="AK3" s="21">
         <v>922337203685477</v>
       </c>
-      <c r="AL3" s="18"/>
-      <c r="AM3" t="s">
+      <c r="AL3" s="17"/>
+      <c r="AM3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AO3" s="19"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" t="s">
+      <c r="AO3" s="18"/>
+      <c r="AP3" s="25"/>
+      <c r="AQ3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AR3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AS3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AU3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AV3">
+      <c r="AV3" s="21">
         <v>10000</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="AX3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="AY3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="AZ3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BA3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BB3" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BC3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BD3" s="20"/>
+      <c r="BD3" s="19"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="A4" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="22" t="s">
@@ -3287,111 +3275,116 @@
       <c r="L4" s="1">
         <v>100</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="21"/>
-      <c r="Q4" s="2" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="20"/>
+      <c r="Q4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="13"/>
-      <c r="U4" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="12"/>
+      <c r="U4" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="V4" s="14"/>
-      <c r="W4" t="s">
+      <c r="V4" s="13"/>
+      <c r="W4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="X4">
-        <v>-2147483647</v>
-      </c>
-      <c r="Y4">
+      <c r="X4" s="21">
+        <v>-2147483648</v>
+      </c>
+      <c r="Y4" s="21">
         <v>2147483647</v>
       </c>
-      <c r="Z4" s="15"/>
-      <c r="AA4">
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="21">
         <v>2</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="21">
         <v>0</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="21">
         <v>1000000000</v>
       </c>
-      <c r="AD4" s="16"/>
-      <c r="AE4">
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="21">
         <v>2</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="21">
         <v>-100000000000</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="21">
         <v>100000000000</v>
       </c>
-      <c r="AH4" s="17"/>
-      <c r="AI4">
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="21">
         <v>2</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="21">
         <v>-922337203685477</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="21">
         <v>922337203685477</v>
       </c>
-      <c r="AL4" s="18"/>
-      <c r="AM4" t="s">
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AN4" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AO4" s="19"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" t="s">
+      <c r="AO4" s="18"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AR4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AS4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AU4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="21">
         <v>10000</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AW4" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AX4" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="AY4" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="AZ4" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BA4" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BB4" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BC4" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BD4" s="20"/>
+      <c r="BD4" s="19"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="A5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="22" t="s">
@@ -3409,105 +3402,105 @@
       <c r="L5" s="1">
         <v>100</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="21"/>
-      <c r="Q5" s="2" t="s">
+      <c r="N5" s="7"/>
+      <c r="O5" s="20"/>
+      <c r="Q5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="13"/>
-      <c r="U5" t="s">
+      <c r="R5" s="6"/>
+      <c r="S5" s="12"/>
+      <c r="U5" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="14"/>
-      <c r="W5" t="s">
+      <c r="V5" s="13"/>
+      <c r="W5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="X5">
-        <v>-2147483647</v>
-      </c>
-      <c r="Y5">
+      <c r="X5" s="21">
+        <v>-2147483648</v>
+      </c>
+      <c r="Y5" s="21">
         <v>2147483647</v>
       </c>
-      <c r="Z5" s="15"/>
-      <c r="AA5">
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="21">
         <v>2</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="21">
         <v>0</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="21">
         <v>1000000000</v>
       </c>
-      <c r="AD5" s="16"/>
-      <c r="AE5">
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="21">
         <v>2</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="21">
         <v>-100000000000</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="21">
         <v>100000000000</v>
       </c>
-      <c r="AH5" s="17"/>
-      <c r="AI5">
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="21">
         <v>2</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="21">
         <v>-922337203685477</v>
       </c>
-      <c r="AK5">
+      <c r="AK5" s="21">
         <v>922337203685477</v>
       </c>
-      <c r="AL5" s="18"/>
-      <c r="AM5" t="s">
+      <c r="AL5" s="17"/>
+      <c r="AM5" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AN5" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" t="s">
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AR5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AS5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AU5" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AV5">
+      <c r="AV5" s="21">
         <v>10000</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AX5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="AY5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="AZ5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BA5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BB5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BC5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BD5" s="20"/>
+      <c r="BD5" s="19"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -3518,6 +3511,13 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="BD1:BD2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -3531,13 +3531,6 @@
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="Uniquement pour les champs textes" sqref="AP3:AP5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -3731,7 +3724,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>X3 X5</xm:sqref>
+          <xm:sqref>X3:X5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="70" id="{77F0BE92-F8E1-469F-A556-B3FC68A62258}">
@@ -4404,22 +4397,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>AM4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="24" id="{1C74CD5C-E982-4EE1-ACF5-D64784CD140A}">
-            <xm:f>D4&lt;&gt;ValidationData!$A$6</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1" tint="0.499984740745262"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>X4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="23" id="{E14925AA-085D-43D0-9918-54334559018A}">
@@ -4986,7 +4963,7 @@
         <v>89</v>
       </c>
       <c r="O1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -5033,7 +5010,7 @@
         <v>90</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
@@ -5080,7 +5057,7 @@
         <v>91</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
@@ -5146,7 +5123,7 @@
         <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
@@ -5162,7 +5139,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
@@ -5170,7 +5147,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated handling of choices to better work with global choices
</commit_message>
<xml_diff>
--- a/Javista.AttributesFactory/Template/Attributes_Template.xlsx
+++ b/Javista.AttributesFactory/Template/Attributes_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\T\Github\Javista.AttributesFactory\Javista.AttributesFactory\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BCC621-9B1D-4DF9-BBD3-FB410BCBC243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387127DA-B5D4-4BB5-959A-AD3DB51FDFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -464,46 +464,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-If </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yes,</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> a global OptionSet will be created and an OptionSet attribute that uses this newly created global OptionSet
-If </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No,</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> an OptionSet attribute will be created with values specified if so, or linked to a global OptionSet if column Values (N) contains the name of an existing global OptionSet
+If this cell is empty, a local choice will be created/updated
+If this cell is not empty, it must contains the name of the global choice
 </t>
         </r>
       </text>
@@ -1110,21 +1072,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Is Global  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Behavior </t>
     </r>
     <r>
@@ -1232,6 +1179,21 @@
   </si>
   <si>
     <t>Whole Number</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Global choice  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1639,6 +1601,78 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1682,78 +1716,6 @@
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -2775,7 +2737,7 @@
   <dimension ref="A1:BJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -2825,118 +2787,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="32" t="s">
+      <c r="A1" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="39" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="41" t="s">
+      <c r="U1" s="62"/>
+      <c r="V1" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="38"/>
-      <c r="V1" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA1" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE1" s="62" t="s">
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI1" s="63" t="s">
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="55" t="s">
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" s="64" t="s">
+      <c r="AM1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="65" t="s">
+      <c r="AN1" s="49"/>
+      <c r="AO1" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="57" t="s">
+      <c r="AP1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="58"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="59"/>
-      <c r="BD1" s="45" t="s">
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AX1" s="43"/>
+      <c r="AY1" s="43"/>
+      <c r="AZ1" s="43"/>
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="43"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="30" t="s">
         <v>10</v>
       </c>
       <c r="BE1" s="27"/>
-      <c r="BF1" s="43" t="s">
-        <v>110</v>
+      <c r="BF1" s="28" t="s">
+        <v>109</v>
       </c>
       <c r="BG1" s="26"/>
       <c r="BH1" s="26"/>
       <c r="BI1" s="26"/>
-      <c r="BJ1" s="44" t="s">
+      <c r="BJ1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:62" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>83</v>
@@ -2948,7 +2910,7 @@
         <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -2977,24 +2939,24 @@
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="40"/>
+      <c r="O2" s="64"/>
       <c r="P2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="42"/>
+      <c r="S2" s="66"/>
       <c r="T2" s="10" t="s">
         <v>30</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="V2" s="48"/>
+      <c r="V2" s="33"/>
       <c r="W2" s="5" t="s">
         <v>98</v>
       </c>
@@ -3004,7 +2966,7 @@
       <c r="Y2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="50"/>
+      <c r="Z2" s="35"/>
       <c r="AA2" s="5" t="s">
         <v>39</v>
       </c>
@@ -3014,7 +2976,7 @@
       <c r="AC2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" s="52"/>
+      <c r="AD2" s="37"/>
       <c r="AE2" s="5" t="s">
         <v>39</v>
       </c>
@@ -3024,7 +2986,7 @@
       <c r="AG2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="54"/>
+      <c r="AH2" s="39"/>
       <c r="AI2" s="5" t="s">
         <v>39</v>
       </c>
@@ -3034,16 +2996,16 @@
       <c r="AK2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="56"/>
+      <c r="AL2" s="41"/>
       <c r="AM2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="66"/>
+      <c r="AO2" s="51"/>
       <c r="AP2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ2" s="4" t="s">
         <v>48</v>
@@ -3084,25 +3046,25 @@
       <c r="BC2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BD2" s="46"/>
+      <c r="BD2" s="31"/>
       <c r="BE2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BF2" s="28"/>
+      <c r="BG2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BH2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BF2" s="43"/>
-      <c r="BG2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BI2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="BI2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="BJ2" s="44"/>
+      <c r="BJ2" s="29"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -3230,7 +3192,7 @@
       <c r="BE3">
         <v>32768</v>
       </c>
-      <c r="BF3" s="43"/>
+      <c r="BF3" s="28"/>
       <c r="BG3">
         <v>10240</v>
       </c>
@@ -3240,11 +3202,11 @@
       <c r="BI3" t="s">
         <v>26</v>
       </c>
-      <c r="BJ3" s="44"/>
+      <c r="BJ3" s="29"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -3371,7 +3333,7 @@
       <c r="BE4">
         <v>32768</v>
       </c>
-      <c r="BF4" s="43"/>
+      <c r="BF4" s="28"/>
       <c r="BG4">
         <v>10240</v>
       </c>
@@ -3381,11 +3343,11 @@
       <c r="BI4" t="s">
         <v>26</v>
       </c>
-      <c r="BJ4" s="44"/>
+      <c r="BJ4" s="29"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -3512,7 +3474,7 @@
       <c r="BE5">
         <v>32768</v>
       </c>
-      <c r="BF5" s="43"/>
+      <c r="BF5" s="28"/>
       <c r="BG5">
         <v>10240</v>
       </c>
@@ -3522,7 +3484,7 @@
       <c r="BI5" t="s">
         <v>26</v>
       </c>
-      <c r="BJ5" s="44"/>
+      <c r="BJ5" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -3533,6 +3495,13 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="22">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="BF1:BF5"/>
     <mergeCell ref="BJ1:BJ5"/>
     <mergeCell ref="BD1:BD2"/>
@@ -3548,13 +3517,6 @@
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="4">
@@ -4844,12 +4806,12 @@
         <v>86</v>
       </c>
       <c r="O1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -4891,12 +4853,12 @@
         <v>87</v>
       </c>
       <c r="O2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4938,7 +4900,7 @@
         <v>88</v>
       </c>
       <c r="O3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -5004,12 +4966,12 @@
         <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -5020,7 +4982,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -5028,7 +4990,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -5068,7 +5030,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
@@ -5123,12 +5085,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>